<commit_message>
Update new feature, Chat demo
</commit_message>
<xml_diff>
--- a/KLTN/KeHoachThucHien.xlsx
+++ b/KLTN/KeHoachThucHien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\KLTN_WebsiteChiaSeHinhAnh_Nhom5_K17\KLTN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Huy Hiep\Desktop\TLCN\KLTN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73D4CBC-895F-42D5-AB96-4FA90774CDA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100EA60D-1D3C-49E8-9BAE-5069A2295A1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{CC123C62-52C6-4428-A23D-0584B9F264F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CC123C62-52C6-4428-A23D-0584B9F264F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>KHOA ĐÀO TẠO CHẤT LƯỢNG CAO</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Dùng code first để hoàn thiện thiết kế database dựa trên sơ đồ quan hệ đã thiết kế.</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -306,9 +309,6 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -322,19 +322,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -361,23 +349,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -695,14 +698,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A12325-C69A-4B93-81B9-79200176B54A}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="37.625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="22.625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="37.625" style="9" customWidth="1"/>
     <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
@@ -713,838 +716,851 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" s="16" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="17" t="s">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="18">
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13">
         <v>44270</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="13">
         <v>44283</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="18">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="13">
         <v>44284</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="13">
         <v>44285</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="23">
         <v>2</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="18">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="13">
         <v>44286</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="13">
         <v>44286</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="7" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="18">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="13">
         <v>44287</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="13">
         <v>44287</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="18">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="13">
         <v>44288</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="13">
         <v>44288</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="23">
         <v>3</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4">
         <v>44289</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>44290</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="7" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4">
         <v>44289</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>44290</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>4</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4">
         <v>44291</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>44291</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>5</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4">
         <v>44292</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>44292</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="23">
         <v>6</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4">
         <v>44293</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>44318</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="7" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="24" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="7" t="s">
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="7" t="s">
+      <c r="A19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4">
+        <v>44292</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="7" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="7" t="s">
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="25" t="s">
+      <c r="A22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="7" t="s">
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="7" t="s">
+      <c r="A24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+      <c r="A28" s="23">
         <v>7</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="5">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4">
         <v>44293</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <v>44318</v>
       </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="7" t="s">
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="24" t="s">
+      <c r="A30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="K30" s="3"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="7" t="s">
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="7" t="s">
+      <c r="A32" s="23"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="7" t="s">
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="7" t="s">
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="25" t="s">
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="7" t="s">
+      <c r="A36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="7" t="s">
+      <c r="A37" s="23"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
     </row>
     <row r="38" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="12" t="s">
+      <c r="A38" s="23"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="5">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="4">
         <v>44319</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="4">
         <v>44346</v>
       </c>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
+      <c r="A40" s="23">
         <v>8</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="5">
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="4">
         <v>44347</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="4">
         <v>44349</v>
       </c>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="7" t="s">
+      <c r="A41" s="23"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="5">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="4">
         <v>44347</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="4">
         <v>44349</v>
       </c>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="7" t="s">
+      <c r="A42" s="23"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="5">
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="4">
         <v>44350</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="4">
         <v>44353</v>
       </c>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="8">
+      <c r="A43" s="20">
         <v>9</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="5">
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="4">
         <v>44354</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G43" s="4">
         <v>44360</v>
       </c>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="7" t="s">
+      <c r="A44" s="21"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="5">
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="4">
         <v>44354</v>
       </c>
-      <c r="G44" s="5">
+      <c r="G44" s="4">
         <v>44360</v>
       </c>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="13" t="s">
+      <c r="A45" s="21"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="5">
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="4">
         <v>44361</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G45" s="4">
         <v>44373</v>
       </c>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="7" t="s">
+      <c r="A46" s="21"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="5">
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="4">
         <v>44374</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G46" s="4">
         <v>44374</v>
       </c>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="7" t="s">
+      <c r="A47" s="22"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="5">
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="4">
         <v>44375</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G47" s="4">
         <v>44375</v>
       </c>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K4"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="B43:B47"/>
     <mergeCell ref="A43:A47"/>
     <mergeCell ref="A15:A27"/>
@@ -1553,13 +1569,6 @@
     <mergeCell ref="B28:B39"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K4"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>